<commit_message>
should be 47uH inductor
</commit_message>
<xml_diff>
--- a/Purchasing_List.xlsx
+++ b/Purchasing_List.xlsx
@@ -347,9 +347,6 @@
     <t>10uF capacitor</t>
   </si>
   <si>
-    <t>4.7uH inductor</t>
-  </si>
-  <si>
     <t xml:space="preserve">5mm LED </t>
   </si>
   <si>
@@ -405,6 +402,9 @@
   </si>
   <si>
     <t>Digikey Part Number: 1276-2552-1-ND</t>
+  </si>
+  <si>
+    <t>47uH inductor</t>
   </si>
 </sst>
 </file>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="172" zoomScaleNormal="172" zoomScalePageLayoutView="172" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="172" zoomScaleNormal="172" zoomScalePageLayoutView="172" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,7 +981,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -995,11 +995,11 @@
     </row>
     <row r="5" spans="2:6" ht="24" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1043,16 +1043,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="24">
-        <v>1</v>
-      </c>
-      <c r="E8" s="25" t="s">
+      <c r="F8" s="25" t="s">
         <v>113</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -1128,16 +1128,16 @@
         <v>7</v>
       </c>
       <c r="C13" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="24">
-        <v>1</v>
-      </c>
-      <c r="E13" s="25" t="s">
+      <c r="F13" s="25" t="s">
         <v>125</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -1162,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="23">
         <v>5</v>
@@ -1247,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D20" s="24">
         <v>1</v>
@@ -1315,7 +1315,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" s="24">
         <v>1</v>
@@ -1451,7 +1451,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="33">
         <v>1</v>
@@ -1525,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F36" s="34" t="s">
         <v>72</v>
@@ -1630,7 +1630,7 @@
         <v>95</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
@@ -1638,13 +1638,13 @@
         <v>37</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D43" s="31">
         <v>1</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F43" s="30" t="s">
         <v>87</v>
@@ -1661,10 +1661,10 @@
         <v>1</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
@@ -1672,7 +1672,7 @@
         <v>39</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D45" s="27">
         <v>1</v>

</xml_diff>

<commit_message>
updated DC Booster part number
</commit_message>
<xml_diff>
--- a/Purchasing_List.xlsx
+++ b/Purchasing_List.xlsx
@@ -200,9 +200,6 @@
     <t>49.9 Ohm resistor</t>
   </si>
   <si>
-    <t>LT3461ES6#TRPBF</t>
-  </si>
-  <si>
     <t>Digikey Part Number: WM17457-ND</t>
   </si>
   <si>
@@ -405,6 +402,9 @@
   </si>
   <si>
     <t>47uH inductor</t>
+  </si>
+  <si>
+    <t>LT3461AES6#PBF</t>
   </si>
 </sst>
 </file>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="172" zoomScaleNormal="172" zoomScalePageLayoutView="172" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="172" zoomScaleNormal="172" zoomScalePageLayoutView="172" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,7 +981,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -995,11 +995,11 @@
     </row>
     <row r="5" spans="2:6" ht="24" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1043,16 +1043,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="24">
-        <v>1</v>
-      </c>
-      <c r="E8" s="25" t="s">
+      <c r="F8" s="25" t="s">
         <v>112</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -1128,16 +1128,16 @@
         <v>7</v>
       </c>
       <c r="C13" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="24">
-        <v>1</v>
-      </c>
-      <c r="E13" s="25" t="s">
+      <c r="F13" s="25" t="s">
         <v>124</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -1145,7 +1145,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" s="24">
         <v>1</v>
@@ -1162,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" s="23">
         <v>5</v>
@@ -1179,7 +1179,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="24">
         <v>1</v>
@@ -1196,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="24">
         <v>1</v>
@@ -1213,7 +1213,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="24">
         <v>1</v>
@@ -1230,7 +1230,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="24">
         <v>1</v>
@@ -1247,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20" s="24">
         <v>1</v>
@@ -1264,7 +1264,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="24">
         <v>2</v>
@@ -1304,10 +1304,10 @@
         <v>1</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
@@ -1315,13 +1315,13 @@
         <v>18</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D24" s="24">
         <v>1</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24" s="25" t="s">
         <v>47</v>
@@ -1366,16 +1366,16 @@
         <v>21</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="6">
         <v>2</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
@@ -1383,16 +1383,16 @@
         <v>22</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="6">
         <v>4</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -1400,16 +1400,16 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" s="6">
         <v>4</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
@@ -1423,7 +1423,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>13</v>
@@ -1434,7 +1434,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="9">
         <v>1</v>
@@ -1451,7 +1451,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="33">
         <v>1</v>
@@ -1485,16 +1485,16 @@
         <v>28</v>
       </c>
       <c r="C34" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="33">
+        <v>1</v>
+      </c>
+      <c r="E34" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="33">
-        <v>1</v>
-      </c>
-      <c r="E34" s="34" t="s">
+      <c r="F34" s="34" t="s">
         <v>64</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" s="35" t="s">
         <v>34</v>
@@ -1519,16 +1519,16 @@
         <v>30</v>
       </c>
       <c r="C36" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="33">
+        <v>1</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="34" t="s">
         <v>71</v>
-      </c>
-      <c r="D36" s="33">
-        <v>1</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
@@ -1536,16 +1536,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="32">
+        <v>1</v>
+      </c>
+      <c r="E37" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="32">
-        <v>1</v>
-      </c>
-      <c r="E37" s="36" t="s">
-        <v>91</v>
-      </c>
       <c r="F37" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
@@ -1553,16 +1553,16 @@
         <v>32</v>
       </c>
       <c r="C38" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="32" t="s">
+      <c r="E38" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="F38" s="34" t="s">
         <v>98</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
@@ -1570,16 +1570,16 @@
         <v>33</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39" s="33">
         <v>4</v>
       </c>
       <c r="E39" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
@@ -1587,16 +1587,16 @@
         <v>34</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="13">
         <v>1</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
@@ -1604,16 +1604,16 @@
         <v>35</v>
       </c>
       <c r="C41" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="16">
+        <v>1</v>
+      </c>
+      <c r="E41" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="16">
-        <v>1</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>86</v>
-      </c>
       <c r="F41" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
@@ -1621,16 +1621,16 @@
         <v>36</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D42" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>95</v>
-      </c>
       <c r="F42" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
@@ -1638,16 +1638,16 @@
         <v>37</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D43" s="31">
         <v>1</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
@@ -1655,16 +1655,16 @@
         <v>38</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" s="27">
         <v>1</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
@@ -1672,16 +1672,16 @@
         <v>39</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D45" s="27">
         <v>1</v>
       </c>
       <c r="E45" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="28" t="s">
         <v>88</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>